<commit_message>
Complete display students-list, upload, download file, read file .xlsx for input-data
</commit_message>
<xml_diff>
--- a/private_html/templates/thong_tin_giao_vien.xlsx
+++ b/private_html/templates/thong_tin_giao_vien.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy Long\Desktop\NCKH\Quản lý sinh viên\quanlysinhvien\private_html\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A897F82D-60EF-4B54-BA19-6AE4710CD917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,95 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="27">
+  <si>
+    <t>9 chữ số</t>
+  </si>
+  <si>
+    <t>Niên khóa</t>
+  </si>
+  <si>
+    <t>Họ tên</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Lớp</t>
+  </si>
+  <si>
+    <t>Khóa</t>
+  </si>
+  <si>
+    <t>Trường</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>CCCD</t>
+  </si>
+  <si>
+    <t>Dân tộc</t>
+  </si>
+  <si>
+    <t>Tôn giáo</t>
+  </si>
+  <si>
+    <t>Quê quán</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>MGV</t>
+  </si>
+  <si>
+    <t>Không ghi khối</t>
+  </si>
+  <si>
+    <t>Đào Duy Long</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>303 Sơn tây</t>
+  </si>
+  <si>
+    <t>0332058965</t>
+  </si>
+  <si>
+    <t>duylongst@gmail.com</t>
+  </si>
+  <si>
+    <t>001203036186</t>
+  </si>
+  <si>
+    <t>Việt Nam</t>
+  </si>
+  <si>
+    <t>Kinh</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Sơn Tây</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +120,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,14 +151,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +468,630 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="13" width="19.6640625" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>211400787</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{527D571A-2330-4F4E-BB92-E06C1D88EDB7}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{0FEAC7FD-051A-48D0-9098-3DE3E57BD7B4}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{1155AACD-273D-484C-8765-5A81FD3D0AC0}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{56D23C0B-D39A-476E-9550-AAF63F43967C}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{C07CEBBB-4BE1-49A4-9B4E-94D1B34DAA18}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{B290B33F-5E6F-4552-A5BF-FCF0E7842E6C}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{67E496C1-406A-416E-AF62-56FF8B7BC047}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{A60C0822-33DD-4443-A336-46575EDEB728}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{D031C544-B4EA-49A6-A547-7BC53E49064D}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{F0986B2B-D279-45C7-A8B0-6597E264A0CD}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{311D131E-18D0-4E04-BE99-02F2761D4A7F}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{997C536F-66D8-4233-9569-F0A9CC1F022B}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{06CDECF2-FCB8-4E5F-BBE4-2A420B0CE565}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>